<commit_message>
- new notebook calculation
</commit_message>
<xml_diff>
--- a/outputs/max_e.xlsx
+++ b/outputs/max_e.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.739698609263685e-16</v>
+        <v>-0.950000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.4050000000000002</v>
+        <v>-3.048814655172414</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -509,7 +509,64 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.3500000000000001</v>
+        <v>-3.007327586206896</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>comb4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.88</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>comb5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.8525</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>comb6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
superstructure improved stress check calculations
</commit_message>
<xml_diff>
--- a/outputs/max_e.xlsx
+++ b/outputs/max_e.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.739698609263685e-16</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.4050000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -503,13 +503,32 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.405</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>comb4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.3500000000000001</v>
+      <c r="E5" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>